<commit_message>
changed the temp and top p
</commit_message>
<xml_diff>
--- a/results/wall_analysis_report.xlsx
+++ b/results/wall_analysis_report.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,7 +461,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>-----------------------------------------------------</t>
+          <t>------------------------------------------</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -481,7 +481,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>-----------</t>
+          <t>-------------</t>
         </is>
       </c>
     </row>
@@ -493,7 +493,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>SW.401: 140mm blockwork wall</t>
+          <t>DW.451: Gypwall Single Frame partition</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -503,17 +503,17 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>140</t>
+          <t>36.00</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>95.00</t>
+          <t>48.00</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>13,300.00</t>
+          <t>1,728.00</t>
         </is>
       </c>
     </row>
@@ -525,7 +525,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>WL.401: Wall lining (Gyproc GypLyner IWL)</t>
+          <t>DW.452: Gypwall Single Frame Enhanced</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -535,17 +535,17 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>110</t>
+          <t>24.00</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>38.00</t>
+          <t>55.00</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>4,180.00</t>
+          <t>1,320.00</t>
         </is>
       </c>
     </row>
@@ -557,7 +557,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>WL.402: Independent wall lining</t>
+          <t>DW.453: Gypwall Single Frame partition</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -567,17 +567,17 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>28</t>
+          <t>18.00</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>44.00</t>
+          <t>60.00</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>1,232.00</t>
+          <t>1,080.00</t>
         </is>
       </c>
     </row>
@@ -589,7 +589,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>WL.404: Thermally insulated independent wall lining</t>
+          <t>SW.401: Medium density blockwork wall</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -599,17 +599,17 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>40</t>
+          <t>45.00</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>52.00</t>
+          <t>75.00</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2,080.00</t>
+          <t>3,375.00</t>
         </is>
       </c>
     </row>
@@ -621,7 +621,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>WL.405: Thermally insulated wall lining</t>
+          <t>WL.401: Wall lining</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -631,17 +631,17 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>60.00</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>60.00</t>
+          <t>40.00</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>960.00</t>
+          <t>2,400.00</t>
         </is>
       </c>
     </row>
@@ -653,7 +653,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>WL.406: Independent wall lining</t>
+          <t>WL.404: Thermally insulated wall lining</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -663,401 +663,17 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>32</t>
+          <t>30.00</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>44.00</t>
+          <t>65.00</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>1,408.00</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>1.7</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>WL.407: Independent wall lining (superloos)</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>48.00</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>576.00</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>1.8</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>WL.408: Ind. wall lining to East Party Wall</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>48.00</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>384.00</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>1.9</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>WL.409: DriLyner Dab lining system</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>32.00</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>256.00</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>1.10</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>DW.451: Gypwall Single Frame, 60min fire</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>36</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>54.00</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>1,944.00</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>1.11</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>DW.452: Gypwall Single Frame Enhanced, 90min fire</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>32</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>62.00</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>1,984.00</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>1.12</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>DW.453: Gypwall Single Frame, 120min fire</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>40</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>68.00</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>2,720.00</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>1.13</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>DW.454: Gypwall Single Frame (pocket doors)</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>58.00</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>464.00</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>1.14</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>SH.451: Shaftwall, 90min fire</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>28</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>65.00</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>1,820.00</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>1.15</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>SH.452: Shaftwall, 120min fire</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>72.00</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>1,152.00</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>1.16</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>SH.453: Shaftwall, 120min fire</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>72.00</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>864.00</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>1.17</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>SW.402: 215mm brickwork (UKPN)</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>120.00</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>720.00</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>1.18</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>VL.401/NL.401/NL.402/NI.404: Misc. wall linings</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>40.00</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>640.00</t>
+          <t>1,950.00</t>
         </is>
       </c>
     </row>

</xml_diff>